<commit_message>
Add anverage word analysis
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t xml:space="preserve">Week </t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>Mead:LP</t>
+  </si>
+  <si>
+    <t>Mead's Average Word Count</t>
+  </si>
+  <si>
+    <t>Response Average Word Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP </t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>Week</t>
   </si>
 </sst>
 </file>
@@ -122,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -145,20 +163,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:L11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,32 +924,43 @@
     <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
     <col min="12" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="21" width="9.140625" style="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="2" t="s">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Z1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="6"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,8 +1018,38 @@
       <c r="T2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1008,8 +1113,44 @@
         <f t="shared" si="0"/>
         <v>2.7685848184752116E-7</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>9</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG3" s="1">
+        <f>TTEST(Z3:Z14,AC3:AC14,1,1)</f>
+        <v>1.6878474485438993E-6</v>
+      </c>
+      <c r="AH3" s="1">
+        <f t="shared" ref="AH3" si="1">TTEST(AA3:AA14,AD3:AD14,1,1)</f>
+        <v>1.3939496379670186E-6</v>
+      </c>
+      <c r="AI3" s="1">
+        <f t="shared" ref="AI3" si="2">TTEST(AB3:AB14,AE3:AE14,1,1)</f>
+        <v>1.0817042530798923E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1058,8 +1199,29 @@
       <c r="P4" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>30</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>31</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1108,8 +1270,29 @@
       <c r="P5" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1158,8 +1341,29 @@
       <c r="P6" s="1">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y6" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1208,8 +1412,29 @@
       <c r="P7" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y7" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>17</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1258,8 +1483,29 @@
       <c r="P8" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y8" s="1">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>16</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>16</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1308,8 +1554,29 @@
       <c r="P9" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y9" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>18</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>24</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1358,8 +1625,29 @@
       <c r="P10" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y10" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>21</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1408,8 +1696,29 @@
       <c r="P11" s="1">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y11" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>32</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>43</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1458,8 +1767,29 @@
       <c r="P12" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y12" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>22</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>27</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1508,8 +1838,29 @@
       <c r="P13" s="1">
         <v>153</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y13" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>9</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>42</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>47</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1558,8 +1909,29 @@
       <c r="P14" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y14" s="1">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>31</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>26</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1608,8 +1980,29 @@
       <c r="P15" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y15" s="1">
+        <v>13</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>16</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1658,8 +2051,29 @@
       <c r="P16" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y16" s="1">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>17</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>16</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1708,8 +2122,29 @@
       <c r="P17" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y17" s="1">
+        <v>15</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>14</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1758,8 +2193,29 @@
       <c r="P18" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y18" s="1">
+        <v>16</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>12</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>17</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1808,8 +2264,29 @@
       <c r="P19" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y19" s="1">
+        <v>17</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>19</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>19</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1858,8 +2335,29 @@
       <c r="P20" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y20" s="1">
+        <v>18</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>19</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1908,8 +2406,29 @@
       <c r="P21" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y21" s="1">
+        <v>19</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>17</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>21</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1958,8 +2477,29 @@
       <c r="P22" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y22" s="1">
+        <v>20</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>14</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>20</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2008,8 +2548,29 @@
       <c r="P23" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y23" s="1">
+        <v>21</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>17</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>11</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2058,8 +2619,29 @@
       <c r="P24" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y24" s="1">
+        <v>22</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>18</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2108,8 +2690,29 @@
       <c r="P25" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y25" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>14</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2158,8 +2761,29 @@
       <c r="P26" s="1">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y26" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>15</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>13</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2208,88 +2832,111 @@
       <c r="P27" s="1">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y27" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>13</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>9</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>36</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f>AVERAGE(E3:E14)</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="F28" s="3">
-        <f t="shared" ref="F28:I28" si="1">AVERAGE(F3:F14)</f>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28:I28" si="3">AVERAGE(F3:F14)</f>
         <v>41.583333333333336</v>
       </c>
-      <c r="G28" s="3">
-        <f t="shared" si="1"/>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
         <v>41.583333333333336</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="1"/>
+      <c r="H28" s="2">
+        <f t="shared" si="3"/>
         <v>4.166666666666667</v>
       </c>
-      <c r="I28" s="3">
-        <f t="shared" si="1"/>
+      <c r="I28" s="2">
+        <f t="shared" si="3"/>
         <v>4.916666666666667</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <f>AVERAGE(J3:J14)</f>
         <v>3.5833333333333335</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f>STDEV(E3:E14)</f>
         <v>3.4200832880164915</v>
       </c>
-      <c r="F29" s="3">
-        <f t="shared" ref="F29:J29" si="2">STDEV(F3:F14)</f>
+      <c r="F29" s="2">
+        <f t="shared" ref="F29:J29" si="4">STDEV(F3:F14)</f>
         <v>3.3967453227875044</v>
       </c>
-      <c r="G29" s="3">
-        <f t="shared" si="2"/>
+      <c r="G29" s="2">
+        <f t="shared" si="4"/>
         <v>3.3967453227875044</v>
       </c>
-      <c r="H29" s="3">
-        <f t="shared" si="2"/>
+      <c r="H29" s="2">
+        <f t="shared" si="4"/>
         <v>2.208797835653566</v>
       </c>
-      <c r="I29" s="3">
-        <f t="shared" si="2"/>
+      <c r="I29" s="2">
+        <f t="shared" si="4"/>
         <v>2.6784776318353725</v>
       </c>
-      <c r="J29" s="3">
-        <f t="shared" si="2"/>
+      <c r="J29" s="2">
+        <f t="shared" si="4"/>
         <v>1.7816403745544227</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <f>CORREL(H3:H14, E3:E14)</f>
         <v>-0.82233215166967744</v>
       </c>
-      <c r="I30" s="3">
-        <f t="shared" ref="I30:J30" si="3">CORREL(I3:I14, F3:F14)</f>
+      <c r="I30" s="2">
+        <f t="shared" ref="I30:J30" si="5">CORREL(I3:I14, F3:F14)</f>
         <v>-0.73358588635800692</v>
       </c>
-      <c r="J30" s="3">
-        <f t="shared" si="3"/>
+      <c r="J30" s="2">
+        <f t="shared" si="5"/>
         <v>-0.4969738570781343</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Z1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished the multi-document evaluation
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -222,6 +219,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,18 +909,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1:AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="10" width="9.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="7" width="15" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="10" width="9.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
     <col min="12" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -929,36 +929,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Z1" s="4" t="s">
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Z1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="4" t="s">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="5"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1103,21 +1103,21 @@
       </c>
       <c r="R3" s="1">
         <f>TTEST(K3:K14,N3:N14,1,1)</f>
-        <v>4.752847749225631E-7</v>
+        <v>4.6654156041070836E-2</v>
       </c>
       <c r="S3" s="1">
         <f t="shared" ref="S3:T3" si="0">TTEST(L3:L14,O3:O14,1,1)</f>
-        <v>2.1697018587636549E-7</v>
+        <v>5.7764620650166715E-2</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" si="0"/>
-        <v>2.7685848184752116E-7</v>
+        <v>4.0879773203309681E-4</v>
       </c>
       <c r="Y3" s="1">
         <v>1</v>
       </c>
       <c r="Z3" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA3" s="1">
         <v>9</v>
@@ -1139,15 +1139,15 @@
       </c>
       <c r="AG3" s="1">
         <f>TTEST(Z3:Z14,AC3:AC14,1,1)</f>
-        <v>1.6878474485438993E-6</v>
+        <v>2.6115188171020555E-6</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" ref="AH3" si="1">TTEST(AA3:AA14,AD3:AD14,1,1)</f>
-        <v>1.3939496379670186E-6</v>
+        <v>8.9041097792401618E-6</v>
       </c>
       <c r="AI3" s="1">
         <f t="shared" ref="AI3" si="2">TTEST(AB3:AB14,AE3:AE14,1,1)</f>
-        <v>1.0817042530798923E-4</v>
+        <v>1.5210142802387952E-4</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -1191,13 +1191,13 @@
         <v>11</v>
       </c>
       <c r="N4" s="1">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="O4" s="1">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="P4" s="1">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="Y4" s="1">
         <v>2</v>
@@ -1212,13 +1212,13 @@
         <v>10</v>
       </c>
       <c r="AC4" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AD4" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AE4" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1262,13 +1262,13 @@
         <v>40</v>
       </c>
       <c r="N5" s="1">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="O5" s="1">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="P5" s="1">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="Y5" s="1">
         <v>3</v>
@@ -1277,19 +1277,19 @@
         <v>9</v>
       </c>
       <c r="AA5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB5" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC5" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AD5" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AE5" s="1">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1333,13 +1333,13 @@
         <v>17</v>
       </c>
       <c r="N6" s="1">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="O6" s="1">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="P6" s="1">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="Y6" s="1">
         <v>4</v>
@@ -1354,13 +1354,13 @@
         <v>8</v>
       </c>
       <c r="AC6" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AD6" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AE6" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -1404,13 +1404,13 @@
         <v>25</v>
       </c>
       <c r="N7" s="1">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="O7" s="1">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P7" s="1">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="Y7" s="1">
         <v>5</v>
@@ -1419,19 +1419,19 @@
         <v>7</v>
       </c>
       <c r="AA7" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB7" s="1">
         <v>7</v>
       </c>
       <c r="AC7" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AD7" s="1">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="AE7" s="1">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -1475,13 +1475,13 @@
         <v>24</v>
       </c>
       <c r="N8" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O8" s="1">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="P8" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y8" s="1">
         <v>6</v>
@@ -1499,7 +1499,7 @@
         <v>16</v>
       </c>
       <c r="AD8" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE8" s="1">
         <v>15</v>
@@ -1546,19 +1546,19 @@
         <v>10</v>
       </c>
       <c r="N9" s="1">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="P9" s="1">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="Y9" s="1">
         <v>7</v>
       </c>
       <c r="Z9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="1">
         <v>7</v>
@@ -1567,13 +1567,13 @@
         <v>11</v>
       </c>
       <c r="AC9" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AD9" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AE9" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
@@ -1617,13 +1617,13 @@
         <v>15</v>
       </c>
       <c r="N10" s="1">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="O10" s="1">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P10" s="1">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="Y10" s="1">
         <v>8</v>
@@ -1632,19 +1632,19 @@
         <v>6</v>
       </c>
       <c r="AA10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB10" s="1">
         <v>6</v>
       </c>
       <c r="AC10" s="1">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="AD10" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AE10" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
@@ -1688,34 +1688,34 @@
         <v>13</v>
       </c>
       <c r="N11" s="1">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="O11" s="1">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="P11" s="1">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Y11" s="1">
         <v>9</v>
       </c>
       <c r="Z11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA11" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB11" s="1">
         <v>8</v>
       </c>
       <c r="AC11" s="1">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="AD11" s="1">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="AE11" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
@@ -1759,34 +1759,34 @@
         <v>22</v>
       </c>
       <c r="N12" s="1">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="O12" s="1">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="P12" s="1">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="1">
         <v>10</v>
       </c>
       <c r="Z12" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA12" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB12" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC12" s="1">
         <v>12</v>
       </c>
-      <c r="AC12" s="1">
-        <v>22</v>
-      </c>
       <c r="AD12" s="1">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="AE12" s="1">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
@@ -1830,34 +1830,34 @@
         <v>84</v>
       </c>
       <c r="N13" s="1">
-        <v>127</v>
+        <v>57</v>
       </c>
       <c r="O13" s="1">
-        <v>141</v>
+        <v>43</v>
       </c>
       <c r="P13" s="1">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="Y13" s="1">
         <v>11</v>
       </c>
       <c r="Z13" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AA13" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AB13" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC13" s="1">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="AD13" s="1">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="AE13" s="1">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -1901,19 +1901,19 @@
         <v>15</v>
       </c>
       <c r="N14" s="1">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="O14" s="1">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="P14" s="1">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="Y14" s="1">
         <v>12</v>
       </c>
       <c r="Z14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA14" s="1">
         <v>10</v>
@@ -1922,13 +1922,13 @@
         <v>8</v>
       </c>
       <c r="AC14" s="1">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="AD14" s="1">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="AE14" s="1">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>